<commit_message>
add function adding address
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BB327F-B8D7-4FC5-803D-806F0F2B72DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Понедельник" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="196">
   <si>
     <t>Название продукта</t>
   </si>
@@ -613,7 +614,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +720,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -735,9 +736,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -775,7 +776,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -810,6 +811,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -845,9 +863,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1020,21 +1055,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1094,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>64</v>
       </c>
@@ -1084,7 +1119,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -1109,7 +1144,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -1134,7 +1169,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>118</v>
       </c>
@@ -1159,7 +1194,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -1184,7 +1219,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -1209,7 +1244,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -1234,7 +1269,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1294,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
@@ -1284,7 +1319,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -1309,7 +1344,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -1334,7 +1369,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>113</v>
       </c>
@@ -1359,7 +1394,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>77</v>
       </c>
@@ -1384,7 +1419,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1409,7 +1444,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1434,7 +1469,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
@@ -1459,7 +1494,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>80</v>
       </c>
@@ -1484,7 +1519,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>81</v>
       </c>
@@ -1509,7 +1544,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>82</v>
       </c>
@@ -1534,7 +1569,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>83</v>
       </c>
@@ -1559,7 +1594,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -1584,7 +1619,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>85</v>
       </c>
@@ -1609,7 +1644,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -1634,7 +1669,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>87</v>
       </c>
@@ -1659,7 +1694,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1676,7 +1711,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
@@ -1693,7 +1728,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
@@ -1710,7 +1745,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -1727,7 +1762,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
@@ -1744,7 +1779,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>90</v>
       </c>
@@ -1761,7 +1796,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>91</v>
       </c>
@@ -1778,7 +1813,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -1795,7 +1830,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>46</v>
       </c>
@@ -1812,7 +1847,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1829,7 +1864,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -1846,7 +1881,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
@@ -1863,7 +1898,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>50</v>
       </c>
@@ -1880,7 +1915,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
@@ -1897,7 +1932,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>53</v>
       </c>
@@ -1914,7 +1949,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>112</v>
       </c>
@@ -1931,7 +1966,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
@@ -1948,7 +1983,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>114</v>
       </c>
@@ -1965,7 +2000,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>58</v>
       </c>
@@ -1982,7 +2017,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -1999,7 +2034,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
@@ -2016,7 +2051,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>120</v>
       </c>
@@ -2040,21 +2075,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2106,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2088,7 +2123,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2105,7 +2140,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2122,7 +2157,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2139,7 +2174,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2156,7 +2191,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2173,7 +2208,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2190,7 +2225,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2207,7 +2242,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2224,7 +2259,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2241,7 +2276,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2258,7 +2293,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2275,7 +2310,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2292,7 +2327,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2309,7 +2344,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2326,7 +2361,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2343,7 +2378,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2360,7 +2395,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2377,7 +2412,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2394,7 +2429,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2411,7 +2446,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2428,7 +2463,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2445,7 +2480,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2462,7 +2497,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2479,7 +2514,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2496,7 +2531,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2513,7 +2548,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2530,7 +2565,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2547,7 +2582,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -2564,7 +2599,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2581,7 +2616,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -2598,7 +2633,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -2615,7 +2650,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
@@ -2632,7 +2667,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2649,7 +2684,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -2666,7 +2701,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -2683,7 +2718,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>60</v>
       </c>
@@ -2700,7 +2735,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -2717,7 +2752,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
@@ -2734,7 +2769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -2751,7 +2786,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
@@ -2768,7 +2803,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
@@ -2785,7 +2820,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -2802,7 +2837,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
@@ -2819,7 +2854,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -2836,7 +2871,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
@@ -2853,7 +2888,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>112</v>
       </c>
@@ -2870,7 +2905,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>56</v>
       </c>
@@ -2887,7 +2922,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -2904,7 +2939,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -2921,7 +2956,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>62</v>
       </c>
@@ -2938,7 +2973,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>63</v>
       </c>
@@ -2955,7 +2990,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>120</v>
       </c>
@@ -2978,21 +3013,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3009,7 +3044,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
@@ -3026,7 +3061,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
@@ -3043,7 +3078,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -3060,7 +3095,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>96</v>
       </c>
@@ -3077,7 +3112,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -3094,7 +3129,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
@@ -3111,7 +3146,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
@@ -3128,7 +3163,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>99</v>
       </c>
@@ -3145,7 +3180,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -3162,7 +3197,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>136</v>
       </c>
@@ -3179,7 +3214,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>103</v>
       </c>
@@ -3196,7 +3231,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -3213,7 +3248,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -3230,7 +3265,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
@@ -3247,7 +3282,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
@@ -3264,7 +3299,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
@@ -3281,7 +3316,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -3298,7 +3333,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>83</v>
       </c>
@@ -3315,7 +3350,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -3332,7 +3367,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>85</v>
       </c>
@@ -3349,7 +3384,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>86</v>
       </c>
@@ -3366,7 +3401,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -3383,7 +3418,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -3400,7 +3435,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>105</v>
       </c>
@@ -3417,7 +3452,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>106</v>
       </c>
@@ -3434,7 +3469,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>107</v>
       </c>
@@ -3451,7 +3486,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>108</v>
       </c>
@@ -3468,7 +3503,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>89</v>
       </c>
@@ -3485,7 +3520,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>109</v>
       </c>
@@ -3502,7 +3537,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>111</v>
       </c>
@@ -3519,7 +3554,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>50</v>
       </c>
@@ -3536,7 +3571,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>110</v>
       </c>
@@ -3553,7 +3588,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>112</v>
       </c>
@@ -3570,7 +3605,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
@@ -3587,7 +3622,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>62</v>
       </c>
@@ -3604,7 +3639,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
@@ -3621,7 +3656,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
@@ -3644,21 +3679,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3675,7 +3710,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>64</v>
       </c>
@@ -3692,7 +3727,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -3709,7 +3744,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -3726,7 +3761,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>118</v>
       </c>
@@ -3743,7 +3778,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -3760,7 +3795,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -3777,7 +3812,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -3794,7 +3829,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -3811,7 +3846,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
@@ -3828,7 +3863,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -3845,7 +3880,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -3862,7 +3897,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>113</v>
       </c>
@@ -3879,7 +3914,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>77</v>
       </c>
@@ -3896,7 +3931,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -3913,7 +3948,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -3930,7 +3965,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
@@ -3947,7 +3982,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>80</v>
       </c>
@@ -3964,7 +3999,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>81</v>
       </c>
@@ -3981,7 +4016,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>82</v>
       </c>
@@ -3998,7 +4033,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>83</v>
       </c>
@@ -4015,7 +4050,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -4032,7 +4067,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>85</v>
       </c>
@@ -4049,7 +4084,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -4066,7 +4101,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>87</v>
       </c>
@@ -4083,7 +4118,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -4100,7 +4135,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
@@ -4117,7 +4152,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
@@ -4134,7 +4169,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -4151,7 +4186,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
@@ -4168,7 +4203,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>90</v>
       </c>
@@ -4185,7 +4220,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>91</v>
       </c>
@@ -4202,7 +4237,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -4219,7 +4254,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>46</v>
       </c>
@@ -4236,7 +4271,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -4253,7 +4288,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -4270,7 +4305,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
@@ -4287,7 +4322,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>50</v>
       </c>
@@ -4304,7 +4339,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
@@ -4321,7 +4356,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>53</v>
       </c>
@@ -4338,7 +4373,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>112</v>
       </c>
@@ -4355,7 +4390,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
@@ -4372,7 +4407,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>114</v>
       </c>
@@ -4389,7 +4424,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>58</v>
       </c>
@@ -4406,7 +4441,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -4423,7 +4458,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
@@ -4440,7 +4475,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>120</v>
       </c>
@@ -4463,7 +4498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
@@ -4471,14 +4506,14 @@
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4495,7 +4530,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4512,7 +4547,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4529,7 +4564,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4546,7 +4581,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4563,7 +4598,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4580,7 +4615,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4597,7 +4632,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -4614,7 +4649,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -4631,7 +4666,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -4648,7 +4683,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -4665,7 +4700,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4682,7 +4717,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -4699,7 +4734,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -4716,7 +4751,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -4733,7 +4768,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -4750,7 +4785,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -4767,7 +4802,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4784,7 +4819,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4801,7 +4836,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -4818,7 +4853,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -4835,7 +4870,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -4852,7 +4887,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -4869,7 +4904,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -4886,7 +4921,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -4903,7 +4938,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -4920,7 +4955,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -4937,7 +4972,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4954,7 +4989,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -4971,7 +5006,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -4988,7 +5023,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -5005,7 +5040,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -5022,7 +5057,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -5039,7 +5074,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
@@ -5056,7 +5091,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -5073,7 +5108,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -5090,7 +5125,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -5107,7 +5142,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>60</v>
       </c>
@@ -5124,7 +5159,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -5141,7 +5176,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
@@ -5158,7 +5193,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -5175,7 +5210,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
@@ -5192,7 +5227,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
@@ -5209,7 +5244,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -5226,7 +5261,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
@@ -5243,7 +5278,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -5260,7 +5295,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
@@ -5277,7 +5312,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>112</v>
       </c>
@@ -5294,7 +5329,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>56</v>
       </c>
@@ -5311,7 +5346,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -5328,7 +5363,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -5345,7 +5380,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>62</v>
       </c>
@@ -5362,7 +5397,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>63</v>
       </c>
@@ -5379,7 +5414,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>120</v>
       </c>
@@ -5396,154 +5431,154 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="7"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
     </row>
   </sheetData>
@@ -5553,21 +5588,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5584,7 +5619,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>64</v>
       </c>
@@ -5601,7 +5636,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -5618,7 +5653,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5635,7 +5670,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>118</v>
       </c>
@@ -5652,7 +5687,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -5669,7 +5704,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -5686,7 +5721,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -5703,12 +5738,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="9">
-        <v>220</v>
+      <c r="B9" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="C9">
         <v>164</v>
@@ -5720,12 +5755,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="9">
-        <v>250</v>
+      <c r="B10" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="C10">
         <v>169</v>
@@ -5737,12 +5772,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="9">
-        <v>400</v>
+      <c r="B11" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="C11">
         <v>198</v>
@@ -5754,12 +5789,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="9">
-        <v>150</v>
+      <c r="B12" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="C12">
         <v>65</v>
@@ -5771,12 +5806,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="9">
-        <v>150</v>
+      <c r="B13" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="C13">
         <v>55</v>
@@ -5788,12 +5823,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="9">
-        <v>150</v>
+      <c r="B14" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="C14">
         <v>80</v>
@@ -5805,7 +5840,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -5822,7 +5857,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -5839,7 +5874,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
@@ -5856,7 +5891,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>80</v>
       </c>
@@ -5873,7 +5908,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>81</v>
       </c>
@@ -5890,7 +5925,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>82</v>
       </c>
@@ -5907,7 +5942,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>83</v>
       </c>
@@ -5924,7 +5959,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -5941,7 +5976,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>85</v>
       </c>
@@ -5958,7 +5993,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -5975,7 +6010,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>87</v>
       </c>
@@ -5992,7 +6027,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -6009,7 +6044,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
@@ -6026,7 +6061,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
@@ -6043,7 +6078,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -6060,7 +6095,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
@@ -6077,7 +6112,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>90</v>
       </c>
@@ -6094,7 +6129,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>91</v>
       </c>
@@ -6111,7 +6146,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -6128,7 +6163,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>46</v>
       </c>
@@ -6145,7 +6180,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -6162,7 +6197,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -6179,7 +6214,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
@@ -6196,7 +6231,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>50</v>
       </c>
@@ -6213,7 +6248,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
@@ -6230,7 +6265,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>53</v>
       </c>
@@ -6247,7 +6282,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>112</v>
       </c>
@@ -6264,7 +6299,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
@@ -6281,7 +6316,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>114</v>
       </c>
@@ -6298,7 +6333,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>58</v>
       </c>
@@ -6315,7 +6350,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -6332,7 +6367,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
@@ -6349,7 +6384,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>120</v>
       </c>
@@ -6372,22 +6407,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="100.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6404,7 +6439,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
@@ -6421,7 +6456,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
@@ -6438,7 +6473,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -6455,7 +6490,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>96</v>
       </c>
@@ -6472,7 +6507,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -6489,7 +6524,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
@@ -6506,7 +6541,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
@@ -6523,7 +6558,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>99</v>
       </c>
@@ -6540,7 +6575,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -6557,7 +6592,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>73</v>
       </c>
@@ -6574,7 +6609,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>103</v>
       </c>
@@ -6591,7 +6626,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -6608,7 +6643,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -6625,7 +6660,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
@@ -6642,7 +6677,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
@@ -6659,7 +6694,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
@@ -6676,7 +6711,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -6693,7 +6728,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>83</v>
       </c>
@@ -6710,7 +6745,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -6727,7 +6762,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>85</v>
       </c>
@@ -6744,7 +6779,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>86</v>
       </c>
@@ -6761,7 +6796,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -6778,7 +6813,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -6795,7 +6830,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>105</v>
       </c>
@@ -6812,7 +6847,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>106</v>
       </c>
@@ -6829,7 +6864,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>107</v>
       </c>
@@ -6846,7 +6881,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>108</v>
       </c>
@@ -6863,7 +6898,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>89</v>
       </c>
@@ -6880,7 +6915,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>109</v>
       </c>
@@ -6897,7 +6932,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>111</v>
       </c>
@@ -6914,7 +6949,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>50</v>
       </c>
@@ -6931,7 +6966,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>110</v>
       </c>
@@ -6948,7 +6983,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>112</v>
       </c>
@@ -6965,7 +7000,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
@@ -6982,7 +7017,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>62</v>
       </c>
@@ -6999,7 +7034,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
@@ -7016,7 +7051,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>

</xml_diff>